<commit_message>
update lates excel file
</commit_message>
<xml_diff>
--- a/WahoClient/wwwroot/OrderDetail.xlsx
+++ b/WahoClient/wwwroot/OrderDetail.xlsx
@@ -20,48 +20,54 @@
     <t>Tên khách hàng:</t>
   </si>
   <si>
-    <t>thu 4</t>
+    <t>aduc00005</t>
   </si>
   <si>
     <t>Tên người giao:</t>
   </si>
   <si>
-    <t>Mai Linh</t>
+    <t>lâm</t>
   </si>
   <si>
     <t>Người tạo:</t>
   </si>
   <si>
-    <t>Nguyễn Tùng Lâm</t>
+    <t>Trần Văn Đức</t>
   </si>
   <si>
     <t>Số điện thoại:</t>
   </si>
   <si>
-    <t>0998888888</t>
-  </si>
-  <si>
-    <t>098756789</t>
+    <t>0354897794</t>
+  </si>
+  <si>
+    <t>0123456789</t>
   </si>
   <si>
     <t>Ngày dự kiến giao:</t>
   </si>
   <si>
-    <t>4/1/2023 12:00:00 AM</t>
+    <t>20/3/2023 12:00:00 AM</t>
   </si>
   <si>
     <t>Email:</t>
   </si>
   <si>
+    <t>aduc00005@gmail.com</t>
+  </si>
+  <si>
     <t>Tình trạng:</t>
   </si>
   <si>
-    <t>Chưa giao hàng</t>
+    <t>Đang giao hàng</t>
   </si>
   <si>
     <t>Mã thuế:</t>
   </si>
   <si>
+    <t>152888</t>
+  </si>
+  <si>
     <t xml:space="preserve">Khu vực: </t>
   </si>
   <si>
@@ -71,7 +77,7 @@
     <t xml:space="preserve">Mã COD: </t>
   </si>
   <si>
-    <t xml:space="preserve">JF199463  </t>
+    <t xml:space="preserve">0999885   </t>
   </si>
   <si>
     <t>Mã sản phẩm</t>
@@ -92,19 +98,13 @@
     <t>Tồn kho</t>
   </si>
   <si>
-    <t xml:space="preserve">Áo Khoác hồng </t>
-  </si>
-  <si>
-    <t>Áo Phông in tất cả LOGO</t>
-  </si>
-  <si>
-    <t>Áo Phông Thêu</t>
-  </si>
-  <si>
-    <t>áo Tshirt ong mật ver 2</t>
-  </si>
-  <si>
-    <t>Áo Khoác hồng</t>
+    <t>Phông trơn</t>
+  </si>
+  <si>
+    <t>Phông xanh dương</t>
+  </si>
+  <si>
+    <t>Phông xanh lá</t>
   </si>
   <si>
     <t xml:space="preserve">Tổng giá tiền: </t>
@@ -159,7 +159,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -170,7 +170,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>1</v>
@@ -215,69 +215,75 @@
       <c r="D3" s="0" t="s">
         <v>12</v>
       </c>
+      <c r="E3" s="0" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" s="0">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D9" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0">
-        <v>300000</v>
+        <v>150000</v>
       </c>
       <c r="F9" s="0">
         <v>100</v>
@@ -285,16 +291,16 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C10" s="0">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D10" s="0">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E10" s="0">
         <v>150000</v>
@@ -305,106 +311,46 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C11" s="0">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D11" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E11" s="0">
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="F11" s="0">
         <v>100</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="0">
-        <v>46</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="0">
-        <v>4</v>
-      </c>
-      <c r="D12" s="0">
-        <v>5</v>
-      </c>
-      <c r="E12" s="0">
-        <v>200000</v>
-      </c>
-      <c r="F12" s="0">
-        <v>100</v>
-      </c>
-    </row>
     <row r="13">
-      <c r="A13" s="0">
-        <v>54</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="0">
-        <v>9</v>
-      </c>
-      <c r="D13" s="0">
-        <v>5</v>
-      </c>
-      <c r="E13" s="0">
-        <v>10000</v>
+      <c r="E13" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="F13" s="0">
-        <v>100</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="0">
-        <v>67</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="0">
-        <v>6</v>
-      </c>
-      <c r="D14" s="0">
-        <v>5</v>
-      </c>
-      <c r="E14" s="0">
-        <v>300000</v>
+      <c r="E14" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="F14" s="0">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="E16" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="0">
-        <v>5453000</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="E17" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="0">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="E18" s="0" t="s">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="0">
-        <v>3453000</v>
+      <c r="F15" s="0">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>